<commit_message>
Major updates -- Commenting
Beta V1.1
</commit_message>
<xml_diff>
--- a/staffTest.xlsx
+++ b/staffTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>position</t>
   </si>
@@ -33,9 +33,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>Bingo</t>
-  </si>
-  <si>
     <t>Tester</t>
   </si>
   <si>
@@ -63,43 +60,43 @@
     <t>godell1</t>
   </si>
   <si>
-    <t>Boom Dyna</t>
-  </si>
-  <si>
-    <t>bdynamite@uca.edu</t>
-  </si>
-  <si>
-    <t>dyan1</t>
-  </si>
-  <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>pls</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>Alison Poteete</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>courses</t>
-  </si>
-  <si>
-    <t>courttest</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>f</t>
+    <t>course 1</t>
+  </si>
+  <si>
+    <t>course 2</t>
+  </si>
+  <si>
+    <t>course 3</t>
+  </si>
+  <si>
+    <t>course 4</t>
+  </si>
+  <si>
+    <t>Bingo Nameo</t>
+  </si>
+  <si>
+    <t>Paul Young</t>
+  </si>
+  <si>
+    <t>pYoung@uca.edu</t>
+  </si>
+  <si>
+    <t>pyoung1</t>
+  </si>
+  <si>
+    <t>youngPass</t>
+  </si>
+  <si>
+    <t>Tracy Martis</t>
+  </si>
+  <si>
+    <t>tmartis1@uca.edu</t>
+  </si>
+  <si>
+    <t>tmartis1</t>
+  </si>
+  <si>
+    <t>2330</t>
   </si>
 </sst>
 </file>
@@ -109,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,6 +129,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -150,10 +155,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -162,8 +171,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -494,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -510,10 +523,10 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -528,7 +541,16 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -536,16 +558,16 @@
         <v>444870</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
       <c r="F2">
         <v>466321</v>
@@ -553,31 +575,31 @@
       <c r="G2" s="3">
         <v>4490</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>1111</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>2222</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>3333</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4">
-        <v>9995</v>
+        <v>111112</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
       <c r="F3">
         <v>122334</v>
@@ -585,190 +607,77 @@
       <c r="G3" s="2">
         <v>3381</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4">
+        <v>111113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>22334</v>
       </c>
+      <c r="G4" s="3">
+        <v>3381</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="4">
-        <v>4334</v>
+        <v>111114</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G5" s="3">
+        <v>4490</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2330</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3331</v>
+      </c>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="4">
-        <v>22211</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4">
-        <v>3453</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4">
-        <v>1902</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4">
-        <v>12234</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4">
-        <v>124456</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10">
-        <v>150</v>
-      </c>
-      <c r="H10">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4">
-        <v>333468</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11">
-        <v>4455</v>
-      </c>
-      <c r="H11">
-        <v>4432</v>
-      </c>
-      <c r="I11">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="4"/>
+      <c r="A6" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>